<commit_message>
add basic proxy support
</commit_message>
<xml_diff>
--- a/doc/amazon_prices.xlsx
+++ b/doc/amazon_prices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="200" windowWidth="33600" windowHeight="19720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="prices" sheetId="1" r:id="rId1"/>
@@ -395,8 +395,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="161">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -570,7 +574,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="161">
+  <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -651,6 +655,8 @@
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -731,6 +737,8 @@
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1064,7 +1072,7 @@
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S32"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
update number of cores on cluster boxes
</commit_message>
<xml_diff>
--- a/doc/amazon_prices.xlsx
+++ b/doc/amazon_prices.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24560" windowHeight="19700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="prices" sheetId="1" r:id="rId1"/>
@@ -300,8 +300,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="271">
+  <cellStyleXfs count="289">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -599,7 +617,7 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="271">
+  <cellStyles count="289">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -735,6 +753,15 @@
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -870,6 +897,15 @@
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1202,8 +1238,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1555,7 +1591,7 @@
         <v>44</v>
       </c>
       <c r="P16" s="6" t="str">
-        <f t="shared" ref="P16:P30" si="5">""""&amp;E16&amp;""" =&gt; "&amp;H16&amp;","</f>
+        <f t="shared" ref="P15:P30" si="5">""""&amp;E16&amp;""" =&gt; "&amp;H16&amp;","</f>
         <v>"m3.large" =&gt; 2,</v>
       </c>
       <c r="Q16" s="6" t="str">
@@ -1740,8 +1776,7 @@
         <v>4</v>
       </c>
       <c r="H20" s="6">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I20" s="10">
         <v>14</v>
@@ -1754,7 +1789,7 @@
       </c>
       <c r="L20" s="13">
         <f t="shared" si="4"/>
-        <v>5.2499999999999998E-2</v>
+        <v>0.105</v>
       </c>
       <c r="N20" s="15" t="s">
         <v>63</v>
@@ -1762,11 +1797,11 @@
       <c r="O20" s="5"/>
       <c r="P20" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>"c3.xlarge" =&gt; 4,</v>
+        <v>"c3.xlarge" =&gt; 2,</v>
       </c>
       <c r="Q20" s="6" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">c3.xlarge,4 Cores,$0.21/hour, - Worker Only - </v>
+        <v xml:space="preserve">c3.xlarge,2 Cores,$0.21/hour, - Worker Only - </v>
       </c>
     </row>
     <row r="21" spans="1:17" s="6" customFormat="1" ht="16">
@@ -1792,8 +1827,7 @@
         <v>8</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I21" s="10">
         <v>28</v>
@@ -1806,7 +1840,7 @@
       </c>
       <c r="L21" s="13">
         <f t="shared" si="4"/>
-        <v>5.2499999999999998E-2</v>
+        <v>0.105</v>
       </c>
       <c r="N21" s="15" t="s">
         <v>63</v>
@@ -1816,11 +1850,11 @@
       </c>
       <c r="P21" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>"c3.2xlarge" =&gt; 8,</v>
+        <v>"c3.2xlarge" =&gt; 4,</v>
       </c>
       <c r="Q21" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>c3.2xlarge,8 Cores,$0.42/hour, - Worker Only - Recommended for Worker</v>
+        <v>c3.2xlarge,4 Cores,$0.42/hour, - Worker Only - Recommended for Worker</v>
       </c>
     </row>
     <row r="22" spans="1:17" s="6" customFormat="1" ht="16">

</xml_diff>

<commit_message>
update scripts to not use sudo. pass in security group option
</commit_message>
<xml_diff>
--- a/doc/amazon_prices.xlsx
+++ b/doc/amazon_prices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="prices" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="65">
   <si>
     <t>General Purpose - Current Generation</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t xml:space="preserve"> - Worker Only</t>
+  </si>
+  <si>
+    <t>Storage</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -276,6 +279,11 @@
       <color rgb="FF333333"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -300,7 +308,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="289">
+  <cellStyleXfs count="303">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -590,8 +598,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -616,8 +638,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="289">
+  <cellStyles count="303">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -762,6 +786,13 @@
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -906,6 +937,13 @@
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1236,10 +1274,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1251,13 +1289,14 @@
     <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
     <col min="12" max="12" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.6640625" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16">
+    <row r="1" spans="1:18" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1288,20 +1327,23 @@
       <c r="L1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16" hidden="1">
+    <row r="2" spans="1:18" ht="16" hidden="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1317,16 +1359,17 @@
         <f t="shared" ref="L2:L9" si="0">IF(H2&lt;&gt;"",B2/H2,"")</f>
         <v/>
       </c>
-      <c r="P2" t="str">
-        <f t="shared" ref="P2:P9" si="1">""""&amp;E2&amp;""" =&gt; "&amp;H2&amp;","</f>
+      <c r="M2" s="4"/>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:Q9" si="1">""""&amp;E2&amp;""" =&gt; "&amp;H2&amp;","</f>
         <v>"" =&gt; ,</v>
       </c>
-      <c r="Q2" t="str">
-        <f t="shared" ref="Q2:Q9" si="2">E2&amp;","&amp;G2&amp;" Cores,"&amp;L2&amp;"/hour,"&amp;O2</f>
+      <c r="R2" t="str">
+        <f t="shared" ref="R2:R9" si="2">E2&amp;","&amp;G2&amp;" Cores,"&amp;L2&amp;"/hour,"&amp;P2</f>
         <v>, Cores,/hour,</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="16" hidden="1">
+    <row r="3" spans="1:18" ht="16" hidden="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1334,16 +1377,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P3" t="str">
+      <c r="M3" s="4"/>
+      <c r="Q3" t="str">
         <f t="shared" si="1"/>
         <v>"" =&gt; ,</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="R3" t="str">
         <f t="shared" si="2"/>
         <v>, Cores,/hour,</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16" hidden="1">
+    <row r="4" spans="1:18" ht="16" hidden="1">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1351,16 +1395,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P4" t="str">
+      <c r="M4" s="4"/>
+      <c r="Q4" t="str">
         <f t="shared" si="1"/>
         <v>"" =&gt; ,</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="R4" t="str">
         <f t="shared" si="2"/>
         <v>, Cores,/hour,</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16" hidden="1">
+    <row r="5" spans="1:18" ht="16" hidden="1">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1376,16 +1421,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P5" t="str">
+      <c r="M5" s="4"/>
+      <c r="Q5" t="str">
         <f t="shared" si="1"/>
         <v>"" =&gt; ,</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="R5" t="str">
         <f t="shared" si="2"/>
         <v>, Cores,/hour,</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16" hidden="1">
+    <row r="6" spans="1:18" ht="16" hidden="1">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1401,16 +1447,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P6" t="str">
+      <c r="M6" s="4"/>
+      <c r="Q6" t="str">
         <f t="shared" si="1"/>
         <v>"" =&gt; ,</v>
       </c>
-      <c r="Q6" t="str">
+      <c r="R6" t="str">
         <f t="shared" si="2"/>
         <v>, Cores,/hour,</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16" hidden="1">
+    <row r="7" spans="1:18" ht="16" hidden="1">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1426,16 +1473,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P7" t="str">
+      <c r="M7" s="4"/>
+      <c r="Q7" t="str">
         <f t="shared" si="1"/>
         <v>"" =&gt; ,</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="R7" t="str">
         <f t="shared" si="2"/>
         <v>, Cores,/hour,</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16" hidden="1">
+    <row r="8" spans="1:18" ht="16" hidden="1">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1453,16 +1501,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P8" t="str">
+      <c r="M8" s="4"/>
+      <c r="Q8" t="str">
         <f t="shared" si="1"/>
         <v>"" =&gt; ,</v>
       </c>
-      <c r="Q8" t="str">
+      <c r="R8" t="str">
         <f t="shared" si="2"/>
         <v>, Cores,/hour,</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="16" hidden="1">
+    <row r="9" spans="1:18" ht="16" hidden="1">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1470,16 +1519,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P9" t="str">
+      <c r="M9" s="4"/>
+      <c r="Q9" t="str">
         <f t="shared" si="1"/>
         <v>"" =&gt; ,</v>
       </c>
-      <c r="Q9" t="str">
+      <c r="R9" t="str">
         <f t="shared" si="2"/>
         <v>, Cores,/hour,</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16" hidden="1">
+    <row r="10" spans="1:18" ht="16" hidden="1">
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
@@ -1489,15 +1539,15 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:17" ht="16" hidden="1">
+    <row r="11" spans="1:18" ht="16" hidden="1">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1"/>
-    <row r="13" spans="1:17" hidden="1"/>
-    <row r="14" spans="1:17" hidden="1"/>
-    <row r="15" spans="1:17" ht="16">
+    <row r="12" spans="1:18" hidden="1"/>
+    <row r="13" spans="1:18" hidden="1"/>
+    <row r="14" spans="1:18" hidden="1"/>
+    <row r="15" spans="1:18" ht="17">
       <c r="A15" s="7" t="s">
         <v>46</v>
       </c>
@@ -1520,7 +1570,7 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H21" si="3">G15</f>
+        <f t="shared" ref="H15:H19" si="3">G15</f>
         <v>1</v>
       </c>
       <c r="I15" s="7">
@@ -1536,19 +1586,23 @@
         <f>IF(H15&lt;&gt;"",B15/H15,"")</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="M15" s="24" t="str">
+        <f>TRIM(LEFT(RIGHT(K15,LEN(K15)-SEARCH("x",K15,1)),3))</f>
+        <v>4</v>
+      </c>
+      <c r="P15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P15" t="str">
+      <c r="Q15" t="str">
         <f>""""&amp;E15&amp;""" =&gt; "&amp;H15&amp;","</f>
         <v>"m3.medium" =&gt; 1,</v>
       </c>
-      <c r="Q15" t="str">
-        <f>E15&amp;","&amp;H15&amp;" Cores,$"&amp;ROUND(B15,2)&amp;"/hour,"&amp;N15&amp;" - "&amp;O15</f>
-        <v>m3.medium,1 Cores,$0.07/hour, - Use only for cluster configuration testing</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" s="6" customFormat="1" ht="16">
+      <c r="R15" t="str">
+        <f>E15&amp;","&amp;H15&amp;" Cores,$"&amp;ROUND(B15,2)&amp;"/hour,"&amp;M15&amp;" GB,"&amp;O15&amp;" - "&amp;P15</f>
+        <v>m3.medium,1 Cores,$0.07/hour,4 GB, - Use only for cluster configuration testing</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A16" s="10" t="s">
         <v>48</v>
       </c>
@@ -1587,19 +1641,23 @@
         <f t="shared" ref="L16:L30" si="4">IF(H16&lt;&gt;"",B16/H16,"")</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="M16" s="25" t="str">
+        <f>TRIM(LEFT(RIGHT(K16,LEN(K16)-SEARCH("x",K16,1)),4))</f>
+        <v>32</v>
+      </c>
+      <c r="P16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="P16" s="6" t="str">
-        <f t="shared" ref="P15:P30" si="5">""""&amp;E16&amp;""" =&gt; "&amp;H16&amp;","</f>
+      <c r="Q16" s="6" t="str">
+        <f t="shared" ref="Q16:Q30" si="5">""""&amp;E16&amp;""" =&gt; "&amp;H16&amp;","</f>
         <v>"m3.large" =&gt; 2,</v>
       </c>
-      <c r="Q16" s="6" t="str">
-        <f t="shared" ref="Q16:Q30" si="6">E16&amp;","&amp;H16&amp;" Cores,$"&amp;ROUND(B16,2)&amp;"/hour,"&amp;N16&amp;" - "&amp;O16</f>
-        <v>m3.large,2 Cores,$0.14/hour, - Recommended for Server</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" s="6" customFormat="1" ht="16">
+      <c r="R16" t="str">
+        <f>E16&amp;","&amp;H16&amp;" Cores,$"&amp;ROUND(B16,2)&amp;"/hour,"&amp;M16&amp;" GB,"&amp;O16&amp;" - "&amp;P16</f>
+        <v>m3.large,2 Cores,$0.14/hour,32 GB, - Recommended for Server</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A17" s="10" t="s">
         <v>1</v>
       </c>
@@ -1638,19 +1696,23 @@
         <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O17" s="5" t="s">
+      <c r="M17" s="25" t="str">
+        <f t="shared" ref="M17:M30" si="6">TRIM(LEFT(RIGHT(K17,LEN(K17)-SEARCH("x",K17,1)),4))</f>
+        <v>40</v>
+      </c>
+      <c r="P17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="P17" s="6" t="str">
+      <c r="Q17" s="6" t="str">
         <f t="shared" si="5"/>
         <v>"m3.xlarge" =&gt; 4,</v>
       </c>
-      <c r="Q17" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>m3.xlarge,4 Cores,$0.28/hour, - Recommended for Server</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" s="6" customFormat="1" ht="16">
+      <c r="R17" t="str">
+        <f>E17&amp;","&amp;H17&amp;" Cores,$"&amp;ROUND(B17,2)&amp;"/hour,"&amp;M17&amp;" GB,"&amp;O17&amp;" - "&amp;P17</f>
+        <v>m3.xlarge,4 Cores,$0.28/hour,40 GB, - Recommended for Server</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A18" s="10" t="s">
         <v>2</v>
       </c>
@@ -1689,19 +1751,23 @@
         <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O18" s="5" t="s">
+      <c r="M18" s="25" t="str">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="P18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="P18" s="6" t="str">
+      <c r="Q18" s="6" t="str">
         <f t="shared" si="5"/>
         <v>"m3.2xlarge" =&gt; 8,</v>
       </c>
-      <c r="Q18" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>m3.2xlarge,8 Cores,$0.56/hour, - Recommended for Server</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" s="6" customFormat="1" ht="16">
+      <c r="R18" t="str">
+        <f>E18&amp;","&amp;H18&amp;" Cores,$"&amp;ROUND(B18,2)&amp;"/hour,"&amp;M18&amp;" GB,"&amp;O18&amp;" - "&amp;P18</f>
+        <v>m3.2xlarge,8 Cores,$0.56/hour,80 GB, - Recommended for Server</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A19" s="10" t="s">
         <v>6</v>
       </c>
@@ -1740,20 +1806,24 @@
         <f t="shared" si="4"/>
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="N19" s="15" t="s">
+      <c r="M19" s="25" t="str">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="O19" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="O19" s="5"/>
-      <c r="P19" s="6" t="str">
+      <c r="P19" s="5"/>
+      <c r="Q19" s="6" t="str">
         <f t="shared" si="5"/>
         <v>"c3.large" =&gt; 2,</v>
       </c>
-      <c r="Q19" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">c3.large,2 Cores,$0.11/hour, - Worker Only - </v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" s="6" customFormat="1" ht="16">
+      <c r="R19" t="str">
+        <f>E19&amp;","&amp;H19&amp;" Cores,$"&amp;ROUND(B19,2)&amp;"/hour,"&amp;M19&amp;" GB,"&amp;O19&amp;" - "&amp;P19</f>
+        <v xml:space="preserve">c3.large,2 Cores,$0.11/hour,16 GB, - Worker Only - </v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A20" s="10" t="s">
         <v>7</v>
       </c>
@@ -1791,20 +1861,24 @@
         <f t="shared" si="4"/>
         <v>0.105</v>
       </c>
-      <c r="N20" s="15" t="s">
+      <c r="M20" s="25" t="str">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="O20" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="O20" s="5"/>
-      <c r="P20" s="6" t="str">
+      <c r="P20" s="5"/>
+      <c r="Q20" s="6" t="str">
         <f t="shared" si="5"/>
         <v>"c3.xlarge" =&gt; 2,</v>
       </c>
-      <c r="Q20" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">c3.xlarge,2 Cores,$0.21/hour, - Worker Only - </v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" s="6" customFormat="1" ht="16">
+      <c r="R20" t="str">
+        <f>E20&amp;","&amp;H20&amp;" Cores,$"&amp;ROUND(B20,2)&amp;"/hour,"&amp;M20&amp;" GB,"&amp;O20&amp;" - "&amp;P20</f>
+        <v xml:space="preserve">c3.xlarge,2 Cores,$0.21/hour,40 GB, - Worker Only - </v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
@@ -1842,22 +1916,26 @@
         <f t="shared" si="4"/>
         <v>0.105</v>
       </c>
-      <c r="N21" s="15" t="s">
+      <c r="M21" s="25" t="str">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="O21" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="O21" s="5" t="s">
+      <c r="P21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="P21" s="6" t="str">
+      <c r="Q21" s="6" t="str">
         <f t="shared" si="5"/>
         <v>"c3.2xlarge" =&gt; 4,</v>
       </c>
-      <c r="Q21" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>c3.2xlarge,4 Cores,$0.42/hour, - Worker Only - Recommended for Worker</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" s="6" customFormat="1" ht="16">
+      <c r="R21" t="str">
+        <f>E21&amp;","&amp;H21&amp;" Cores,$"&amp;ROUND(B21,2)&amp;"/hour,"&amp;M21&amp;" GB,"&amp;O21&amp;" - "&amp;P21</f>
+        <v>c3.2xlarge,4 Cores,$0.42/hour,80 GB, - Worker Only - Recommended for Worker</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A22" s="10" t="s">
         <v>9</v>
       </c>
@@ -1895,25 +1973,29 @@
         <f t="shared" si="4"/>
         <v>0.105</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M22" s="25" t="str">
+        <f t="shared" si="6"/>
+        <v>160</v>
+      </c>
+      <c r="N22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N22" s="15" t="s">
+      <c r="O22" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="O22" s="5" t="s">
+      <c r="P22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="P22" s="6" t="str">
+      <c r="Q22" s="6" t="str">
         <f t="shared" si="5"/>
         <v>"c3.4xlarge" =&gt; 8,</v>
       </c>
-      <c r="Q22" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>c3.4xlarge,8 Cores,$0.84/hour, - Worker Only - Recommended for Worker</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" s="6" customFormat="1" ht="16">
+      <c r="R22" t="str">
+        <f>E22&amp;","&amp;H22&amp;" Cores,$"&amp;ROUND(B22,2)&amp;"/hour,"&amp;M22&amp;" GB,"&amp;O22&amp;" - "&amp;P22</f>
+        <v>c3.4xlarge,8 Cores,$0.84/hour,160 GB, - Worker Only - Recommended for Worker</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A23" s="10" t="s">
         <v>10</v>
       </c>
@@ -1951,25 +2033,29 @@
         <f t="shared" si="4"/>
         <v>0.105</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="M23" s="25" t="str">
+        <f t="shared" si="6"/>
+        <v>320</v>
+      </c>
+      <c r="N23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N23" s="15" t="s">
+      <c r="O23" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="O23" s="5" t="s">
+      <c r="P23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="P23" s="6" t="str">
+      <c r="Q23" s="6" t="str">
         <f t="shared" si="5"/>
         <v>"c3.8xlarge" =&gt; 16,</v>
       </c>
-      <c r="Q23" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>c3.8xlarge,16 Cores,$1.68/hour, - Worker Only - Recommended for Worker</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" s="19" customFormat="1" ht="16">
+      <c r="R23" t="str">
+        <f>E23&amp;","&amp;H23&amp;" Cores,$"&amp;ROUND(B23,2)&amp;"/hour,"&amp;M23&amp;" GB,"&amp;O23&amp;" - "&amp;P23</f>
+        <v>c3.8xlarge,16 Cores,$1.68/hour,320 GB, - Worker Only - Recommended for Worker</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="19" customFormat="1" ht="17">
       <c r="A24" s="17" t="s">
         <v>53</v>
       </c>
@@ -2008,17 +2094,21 @@
         <f t="shared" si="4"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="N24" s="21"/>
-      <c r="P24" s="19" t="str">
+      <c r="M24" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="O24" s="21"/>
+      <c r="Q24" s="19" t="str">
         <f t="shared" si="5"/>
         <v>"r3.large" =&gt; 2,</v>
       </c>
-      <c r="Q24" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">r3.large,2 Cores,$0.18/hour, - </v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" s="19" customFormat="1" ht="16">
+      <c r="R24" t="str">
+        <f>E24&amp;","&amp;H24&amp;" Cores,$"&amp;ROUND(B24,2)&amp;"/hour,"&amp;M24&amp;" GB,"&amp;O24&amp;" - "&amp;P24</f>
+        <v xml:space="preserve">r3.large,2 Cores,$0.18/hour,32 GB, - </v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="19" customFormat="1" ht="17">
       <c r="A25" s="17" t="s">
         <v>54</v>
       </c>
@@ -2057,17 +2147,21 @@
         <f t="shared" si="4"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="N25" s="21"/>
-      <c r="P25" s="19" t="str">
+      <c r="M25" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="O25" s="21"/>
+      <c r="Q25" s="19" t="str">
         <f t="shared" si="5"/>
         <v>"r3.xlarge" =&gt; 4,</v>
       </c>
-      <c r="Q25" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">r3.xlarge,4 Cores,$0.35/hour, - </v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" s="19" customFormat="1" ht="16">
+      <c r="R25" t="str">
+        <f>E25&amp;","&amp;H25&amp;" Cores,$"&amp;ROUND(B25,2)&amp;"/hour,"&amp;M25&amp;" GB,"&amp;O25&amp;" - "&amp;P25</f>
+        <v xml:space="preserve">r3.xlarge,4 Cores,$0.35/hour,80 GB, - </v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" s="19" customFormat="1" ht="17">
       <c r="A26" s="17" t="s">
         <v>56</v>
       </c>
@@ -2106,17 +2200,21 @@
         <f t="shared" si="4"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="N26" s="21"/>
-      <c r="P26" s="19" t="str">
+      <c r="M26" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>160</v>
+      </c>
+      <c r="O26" s="21"/>
+      <c r="Q26" s="19" t="str">
         <f t="shared" si="5"/>
         <v>"r3.2xlarge" =&gt; 8,</v>
       </c>
-      <c r="Q26" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">r3.2xlarge,8 Cores,$0.7/hour, - </v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" s="19" customFormat="1" ht="16">
+      <c r="R26" t="str">
+        <f>E26&amp;","&amp;H26&amp;" Cores,$"&amp;ROUND(B26,2)&amp;"/hour,"&amp;M26&amp;" GB,"&amp;O26&amp;" - "&amp;P26</f>
+        <v xml:space="preserve">r3.2xlarge,8 Cores,$0.7/hour,160 GB, - </v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="19" customFormat="1" ht="17">
       <c r="A27" s="17" t="s">
         <v>58</v>
       </c>
@@ -2154,19 +2252,23 @@
         <f t="shared" si="4"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="M27" s="21" t="s">
+      <c r="M27" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>320</v>
+      </c>
+      <c r="N27" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="P27" s="19" t="str">
+      <c r="Q27" s="19" t="str">
         <f t="shared" si="5"/>
         <v>"r3.4xlarge" =&gt; 16,</v>
       </c>
-      <c r="Q27" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">r3.4xlarge,16 Cores,$1.4/hour, - </v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" s="19" customFormat="1" ht="16">
+      <c r="R27" t="str">
+        <f>E27&amp;","&amp;H27&amp;" Cores,$"&amp;ROUND(B27,2)&amp;"/hour,"&amp;M27&amp;" GB,"&amp;O27&amp;" - "&amp;P27</f>
+        <v xml:space="preserve">r3.4xlarge,16 Cores,$1.4/hour,320 GB, - </v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="19" customFormat="1" ht="17">
       <c r="A28" s="17" t="s">
         <v>60</v>
       </c>
@@ -2204,19 +2306,23 @@
         <f t="shared" si="4"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="M28" s="21" t="s">
+      <c r="M28" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>320</v>
+      </c>
+      <c r="N28" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="P28" s="19" t="str">
+      <c r="Q28" s="19" t="str">
         <f t="shared" si="5"/>
         <v>"r3.8xlarge" =&gt; 32,</v>
       </c>
-      <c r="Q28" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">r3.8xlarge,32 Cores,$2.8/hour, - </v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" s="6" customFormat="1" ht="16">
+      <c r="R28" t="str">
+        <f>E28&amp;","&amp;H28&amp;" Cores,$"&amp;ROUND(B28,2)&amp;"/hour,"&amp;M28&amp;" GB,"&amp;O28&amp;" - "&amp;P28</f>
+        <v xml:space="preserve">r3.8xlarge,32 Cores,$2.8/hour,320 GB, - </v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A29" s="10" t="s">
         <v>17</v>
       </c>
@@ -2254,19 +2360,22 @@
         <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
-      <c r="O29" s="16" t="s">
+      <c r="M29" s="25">
+        <v>0</v>
+      </c>
+      <c r="P29" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="P29" s="6" t="str">
+      <c r="Q29" s="6" t="str">
         <f t="shared" si="5"/>
         <v>"t1.micro" =&gt; 1,</v>
       </c>
-      <c r="Q29" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>t1.micro,1 Cores,$0.02/hour, - Use only for cluster configuration testing</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="16">
+      <c r="R29" t="str">
+        <f>E29&amp;","&amp;H29&amp;" Cores,$"&amp;ROUND(B29,2)&amp;"/hour,"&amp;M29&amp;" GB,"&amp;O29&amp;" - "&amp;P29</f>
+        <v>t1.micro,1 Cores,$0.02/hour,0 GB, - Use only for cluster configuration testing</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="17">
       <c r="A30" s="7" t="s">
         <v>4</v>
       </c>
@@ -2304,16 +2413,20 @@
         <f t="shared" si="4"/>
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="O30" s="3" t="s">
+      <c r="M30" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>160</v>
+      </c>
+      <c r="P30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P30" t="str">
+      <c r="Q30" t="str">
         <f t="shared" si="5"/>
         <v>"m1.small" =&gt; 1,</v>
       </c>
-      <c r="Q30" t="str">
-        <f t="shared" si="6"/>
-        <v>m1.small,1 Cores,$0.04/hour, - Use only for cluster configuration testing</v>
+      <c r="R30" t="str">
+        <f>E30&amp;","&amp;H30&amp;" Cores,$"&amp;ROUND(B30,2)&amp;"/hour,"&amp;M30&amp;" GB,"&amp;O30&amp;" - "&amp;P30</f>
+        <v>m1.small,1 Cores,$0.04/hour,160 GB, - Use only for cluster configuration testing</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cores and pricing in spreadsheet
</commit_message>
<xml_diff>
--- a/doc/amazon_prices.xlsx
+++ b/doc/amazon_prices.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="prices" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="72">
   <si>
     <t>General Purpose - Current Generation</t>
   </si>
@@ -217,6 +217,27 @@
   </si>
   <si>
     <t>Storage</t>
+  </si>
+  <si>
+    <t>m2.2xlarge</t>
+  </si>
+  <si>
+    <t>1 x 850</t>
+  </si>
+  <si>
+    <t>m2.4xlarge</t>
+  </si>
+  <si>
+    <t>2 x 840</t>
+  </si>
+  <si>
+    <t>Recommended for Server if large analysis because of storage</t>
+  </si>
+  <si>
+    <t>Display Notes</t>
+  </si>
+  <si>
+    <t>Keep this available until we are able to mount EBS dynamically because the m3 instances have limited size SSD.</t>
   </si>
 </sst>
 </file>
@@ -226,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -257,14 +278,6 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -308,7 +321,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="303">
+  <cellStyleXfs count="369">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -612,8 +625,74 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -621,27 +700,48 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="303">
+  <cellStyles count="369">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -793,6 +893,39 @@
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -944,6 +1077,39 @@
     <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1274,10 +1440,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="R15" sqref="R15:R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1290,8 +1456,8 @@
     <col min="11" max="11" width="16" customWidth="1"/>
     <col min="12" max="12" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.6640625" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.1640625" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="42.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1330,11 +1496,14 @@
       <c r="M1" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="O1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>38</v>
@@ -1570,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H19" si="3">G15</f>
+        <f t="shared" ref="H15:H25" si="3">G15</f>
         <v>1</v>
       </c>
       <c r="I15" s="7">
@@ -1586,11 +1755,13 @@
         <f>IF(H15&lt;&gt;"",B15/H15,"")</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M15" s="24" t="str">
+      <c r="M15" s="21" t="str">
         <f>TRIM(LEFT(RIGHT(K15,LEN(K15)-SEARCH("x",K15,1)),3))</f>
         <v>4</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="25" t="s">
         <v>42</v>
       </c>
       <c r="Q15" t="str">
@@ -1598,7 +1769,7 @@
         <v>"m3.medium" =&gt; 1,</v>
       </c>
       <c r="R15" t="str">
-        <f>E15&amp;","&amp;H15&amp;" Cores,$"&amp;ROUND(B15,2)&amp;"/hour,"&amp;M15&amp;" GB,"&amp;O15&amp;" - "&amp;P15</f>
+        <f t="shared" ref="R15:R32" si="4">E15&amp;","&amp;H15&amp;" Cores,$"&amp;ROUND(B15,2)&amp;"/hour,"&amp;M15&amp;" GB,"&amp;O15&amp;" - "&amp;P15</f>
         <v>m3.medium,1 Cores,$0.07/hour,4 GB, - Use only for cluster configuration testing</v>
       </c>
     </row>
@@ -1638,22 +1809,24 @@
         <v>49</v>
       </c>
       <c r="L16" s="13">
-        <f t="shared" ref="L16:L30" si="4">IF(H16&lt;&gt;"",B16/H16,"")</f>
+        <f t="shared" ref="L16:L32" si="5">IF(H16&lt;&gt;"",B16/H16,"")</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M16" s="25" t="str">
+      <c r="M16" s="22" t="str">
         <f>TRIM(LEFT(RIGHT(K16,LEN(K16)-SEARCH("x",K16,1)),4))</f>
         <v>32</v>
       </c>
-      <c r="P16" s="5" t="s">
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q16" s="6" t="str">
-        <f t="shared" ref="Q16:Q30" si="5">""""&amp;E16&amp;""" =&gt; "&amp;H16&amp;","</f>
+        <f t="shared" ref="Q16:Q32" si="6">""""&amp;E16&amp;""" =&gt; "&amp;H16&amp;","</f>
         <v>"m3.large" =&gt; 2,</v>
       </c>
       <c r="R16" t="str">
-        <f>E16&amp;","&amp;H16&amp;" Cores,$"&amp;ROUND(B16,2)&amp;"/hour,"&amp;M16&amp;" GB,"&amp;O16&amp;" - "&amp;P16</f>
+        <f t="shared" si="4"/>
         <v>m3.large,2 Cores,$0.14/hour,32 GB, - Recommended for Server</v>
       </c>
     </row>
@@ -1693,22 +1866,24 @@
         <v>28</v>
       </c>
       <c r="L17" s="13">
+        <f t="shared" si="5"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M17" s="22" t="str">
+        <f t="shared" ref="M17:M32" si="7">TRIM(LEFT(RIGHT(K17,LEN(K17)-SEARCH("x",K17,1)),4))</f>
+        <v>40</v>
+      </c>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q17" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>"m3.xlarge" =&gt; 4,</v>
+      </c>
+      <c r="R17" t="str">
         <f t="shared" si="4"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="M17" s="25" t="str">
-        <f t="shared" ref="M17:M30" si="6">TRIM(LEFT(RIGHT(K17,LEN(K17)-SEARCH("x",K17,1)),4))</f>
-        <v>40</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q17" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>"m3.xlarge" =&gt; 4,</v>
-      </c>
-      <c r="R17" t="str">
-        <f>E17&amp;","&amp;H17&amp;" Cores,$"&amp;ROUND(B17,2)&amp;"/hour,"&amp;M17&amp;" GB,"&amp;O17&amp;" - "&amp;P17</f>
         <v>m3.xlarge,4 Cores,$0.28/hour,40 GB, - Recommended for Server</v>
       </c>
     </row>
@@ -1748,199 +1923,208 @@
         <v>29</v>
       </c>
       <c r="L18" s="13">
+        <f t="shared" si="5"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M18" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q18" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>"m3.2xlarge" =&gt; 8,</v>
+      </c>
+      <c r="R18" t="str">
         <f t="shared" si="4"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="M18" s="25" t="str">
-        <f t="shared" si="6"/>
-        <v>80</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q18" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>"m3.2xlarge" =&gt; 8,</v>
-      </c>
-      <c r="R18" t="str">
-        <f>E18&amp;","&amp;H18&amp;" Cores,$"&amp;ROUND(B18,2)&amp;"/hour,"&amp;M18&amp;" GB,"&amp;O18&amp;" - "&amp;P18</f>
         <v>m3.2xlarge,8 Cores,$0.56/hour,80 GB, - Recommended for Server</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="6" customFormat="1" ht="17">
+    <row r="19" spans="1:18" s="6" customFormat="1" ht="48">
       <c r="A19" s="10" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B19" s="11">
-        <v>0.105</v>
+        <v>0.49</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G19" s="10">
+        <v>4</v>
+      </c>
+      <c r="H19" s="6">
+        <f>G19</f>
+        <v>4</v>
+      </c>
+      <c r="I19" s="7">
+        <v>13</v>
+      </c>
+      <c r="J19" s="7">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="13">
+        <f>IF(H19&lt;&gt;"",B19/H19,"")</f>
+        <v>0.1225</v>
+      </c>
+      <c r="M19" s="22" t="str">
+        <f>TRIM(LEFT(RIGHT(K19,LEN(K19)-SEARCH("x",K19,1)),4))</f>
+        <v>850</v>
+      </c>
+      <c r="N19" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q19" s="6" t="str">
+        <f>""""&amp;E19&amp;""" =&gt; "&amp;H19&amp;","</f>
+        <v>"m2.2xlarge" =&gt; 4,</v>
+      </c>
+      <c r="R19" t="str">
+        <f>E19&amp;","&amp;H19&amp;" Cores,$"&amp;ROUND(B19,2)&amp;"/hour,"&amp;M19&amp;" GB,"&amp;O19&amp;" - "&amp;P19</f>
+        <v>m2.2xlarge,4 Cores,$0.49/hour,850 GB, - Recommended for Server if large analysis because of storage</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="6" customFormat="1" ht="48">
+      <c r="A20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="11">
+        <v>0.98</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="10">
+        <v>8</v>
+      </c>
+      <c r="H20" s="6">
+        <f>G20</f>
+        <v>8</v>
+      </c>
+      <c r="I20" s="7">
+        <v>26</v>
+      </c>
+      <c r="J20" s="7">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="13">
+        <f>IF(H20&lt;&gt;"",B20/H20,"")</f>
+        <v>0.1225</v>
+      </c>
+      <c r="M20" s="22" t="str">
+        <f>TRIM(LEFT(RIGHT(K20,LEN(K20)-SEARCH("x",K20,1)),4))</f>
+        <v>840</v>
+      </c>
+      <c r="N20" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q20" s="6" t="str">
+        <f>""""&amp;E20&amp;""" =&gt; "&amp;H20&amp;","</f>
+        <v>"m2.4xlarge" =&gt; 8,</v>
+      </c>
+      <c r="R20" t="str">
+        <f>E20&amp;","&amp;H20&amp;" Cores,$"&amp;ROUND(B20,2)&amp;"/hour,"&amp;M20&amp;" GB,"&amp;O20&amp;" - "&amp;P20</f>
+        <v>m2.4xlarge,8 Cores,$0.98/hour,840 GB, - Recommended for Server if large analysis because of storage</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="6" customFormat="1" ht="17">
+      <c r="A21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="11">
+        <v>0.105</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="10">
         <v>2</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H21" s="6">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I21" s="10">
         <v>7</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J21" s="10">
         <v>3.75</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L21" s="13">
+        <f t="shared" si="5"/>
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="M21" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="N21" s="26"/>
+      <c r="O21" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>"c3.large" =&gt; 2,</v>
+      </c>
+      <c r="R21" t="str">
         <f t="shared" si="4"/>
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="M19" s="25" t="str">
-        <f t="shared" si="6"/>
-        <v>16</v>
-      </c>
-      <c r="O19" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>"c3.large" =&gt; 2,</v>
-      </c>
-      <c r="R19" t="str">
-        <f>E19&amp;","&amp;H19&amp;" Cores,$"&amp;ROUND(B19,2)&amp;"/hour,"&amp;M19&amp;" GB,"&amp;O19&amp;" - "&amp;P19</f>
         <v xml:space="preserve">c3.large,2 Cores,$0.11/hour,16 GB, - Worker Only - </v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" s="6" customFormat="1" ht="17">
-      <c r="A20" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="11">
-        <v>0.21</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="10">
-        <v>4</v>
-      </c>
-      <c r="H20" s="6">
-        <v>2</v>
-      </c>
-      <c r="I20" s="10">
-        <v>14</v>
-      </c>
-      <c r="J20" s="10">
-        <v>7.5</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L20" s="13">
-        <f t="shared" si="4"/>
-        <v>0.105</v>
-      </c>
-      <c r="M20" s="25" t="str">
-        <f t="shared" si="6"/>
-        <v>40</v>
-      </c>
-      <c r="O20" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>"c3.xlarge" =&gt; 2,</v>
-      </c>
-      <c r="R20" t="str">
-        <f>E20&amp;","&amp;H20&amp;" Cores,$"&amp;ROUND(B20,2)&amp;"/hour,"&amp;M20&amp;" GB,"&amp;O20&amp;" - "&amp;P20</f>
-        <v xml:space="preserve">c3.xlarge,2 Cores,$0.21/hour,40 GB, - Worker Only - </v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" s="6" customFormat="1" ht="17">
-      <c r="A21" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="11">
-        <v>0.42</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="10">
-        <v>8</v>
-      </c>
-      <c r="H21" s="6">
-        <v>4</v>
-      </c>
-      <c r="I21" s="10">
-        <v>28</v>
-      </c>
-      <c r="J21" s="10">
-        <v>15</v>
-      </c>
-      <c r="K21" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L21" s="13">
-        <f t="shared" si="4"/>
-        <v>0.105</v>
-      </c>
-      <c r="M21" s="25" t="str">
-        <f t="shared" si="6"/>
-        <v>80</v>
-      </c>
-      <c r="O21" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="P21" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q21" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>"c3.2xlarge" =&gt; 4,</v>
-      </c>
-      <c r="R21" t="str">
-        <f>E21&amp;","&amp;H21&amp;" Cores,$"&amp;ROUND(B21,2)&amp;"/hour,"&amp;M21&amp;" GB,"&amp;O21&amp;" - "&amp;P21</f>
-        <v>c3.2xlarge,4 Cores,$0.42/hour,80 GB, - Worker Only - Recommended for Worker</v>
       </c>
     </row>
     <row r="22" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A22" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="11">
-        <v>0.84</v>
+        <v>0.21</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>35</v>
@@ -1949,58 +2133,55 @@
         <v>51</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G22" s="10">
-        <v>16</v>
-      </c>
-      <c r="H22" s="14">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="H22" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="I22" s="10">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="J22" s="10">
-        <v>30</v>
+        <v>7.5</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L22" s="13">
+        <f t="shared" si="5"/>
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="M22" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="N22" s="26"/>
+      <c r="O22" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>"c3.xlarge" =&gt; 4,</v>
+      </c>
+      <c r="R22" t="str">
         <f t="shared" si="4"/>
-        <v>0.105</v>
-      </c>
-      <c r="M22" s="25" t="str">
-        <f t="shared" si="6"/>
-        <v>160</v>
-      </c>
-      <c r="N22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="O22" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q22" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>"c3.4xlarge" =&gt; 8,</v>
-      </c>
-      <c r="R22" t="str">
-        <f>E22&amp;","&amp;H22&amp;" Cores,$"&amp;ROUND(B22,2)&amp;"/hour,"&amp;M22&amp;" GB,"&amp;O22&amp;" - "&amp;P22</f>
-        <v>c3.4xlarge,8 Cores,$0.84/hour,160 GB, - Worker Only - Recommended for Worker</v>
+        <v xml:space="preserve">c3.xlarge,4 Cores,$0.21/hour,40 GB, - Worker Only - </v>
       </c>
     </row>
     <row r="23" spans="1:18" s="6" customFormat="1" ht="17">
       <c r="A23" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B23" s="11">
-        <v>1.68</v>
+        <v>0.42</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>35</v>
@@ -2009,425 +2190,586 @@
         <v>51</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G23" s="10">
+        <v>8</v>
+      </c>
+      <c r="H23" s="6">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I23" s="10">
+        <v>28</v>
+      </c>
+      <c r="J23" s="10">
+        <v>15</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L23" s="13">
+        <f t="shared" si="5"/>
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="M23" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
+      <c r="N23" s="26"/>
+      <c r="O23" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="P23" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q23" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>"c3.2xlarge" =&gt; 8,</v>
+      </c>
+      <c r="R23" t="str">
+        <f t="shared" si="4"/>
+        <v>c3.2xlarge,8 Cores,$0.42/hour,80 GB, - Worker Only - Recommended for Worker</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="6" customFormat="1" ht="17">
+      <c r="A24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="11">
+        <v>0.84</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="10">
+        <v>16</v>
+      </c>
+      <c r="H24" s="6">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I24" s="10">
+        <v>55</v>
+      </c>
+      <c r="J24" s="10">
+        <v>30</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L24" s="13">
+        <f t="shared" si="5"/>
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="M24" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>160</v>
+      </c>
+      <c r="N24" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="O24" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="P24" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q24" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>"c3.4xlarge" =&gt; 16,</v>
+      </c>
+      <c r="R24" t="str">
+        <f t="shared" si="4"/>
+        <v>c3.4xlarge,16 Cores,$0.84/hour,160 GB, - Worker Only - Recommended for Worker</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="6" customFormat="1" ht="17">
+      <c r="A25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="11">
+        <v>1.68</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="10">
         <v>32</v>
       </c>
-      <c r="H23" s="14">
+      <c r="H25" s="6">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="I25" s="10">
+        <v>108</v>
+      </c>
+      <c r="J25" s="10">
+        <v>60</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L25" s="13">
+        <f t="shared" si="5"/>
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="M25" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>320</v>
+      </c>
+      <c r="N25" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="O25" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="P25" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q25" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>"c3.8xlarge" =&gt; 32,</v>
+      </c>
+      <c r="R25" t="str">
+        <f t="shared" si="4"/>
+        <v>c3.8xlarge,32 Cores,$1.68/hour,320 GB, - Worker Only - Recommended for Worker</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" s="17" customFormat="1" ht="17">
+      <c r="A26" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="16">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="15">
+        <v>2</v>
+      </c>
+      <c r="H26" s="17">
+        <f>G26</f>
+        <v>2</v>
+      </c>
+      <c r="I26" s="15">
+        <v>6.5</v>
+      </c>
+      <c r="J26" s="15">
+        <v>15</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="L26" s="20">
+        <f t="shared" si="5"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="M26" s="21" t="str">
+        <f t="shared" si="7"/>
+        <v>32</v>
+      </c>
+      <c r="N26" s="29"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v>"r3.large" =&gt; 2,</v>
+      </c>
+      <c r="R26" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">r3.large,2 Cores,$0.18/hour,32 GB, - </v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="17" customFormat="1" ht="17">
+      <c r="A27" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="15">
+        <v>4</v>
+      </c>
+      <c r="H27" s="17">
+        <f>G27</f>
+        <v>4</v>
+      </c>
+      <c r="I27" s="15">
+        <v>13</v>
+      </c>
+      <c r="J27" s="15">
+        <v>30.5</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L27" s="20">
+        <f t="shared" si="5"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="M27" s="21" t="str">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
+      <c r="N27" s="29"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v>"r3.xlarge" =&gt; 4,</v>
+      </c>
+      <c r="R27" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">r3.xlarge,4 Cores,$0.35/hour,80 GB, - </v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="17" customFormat="1" ht="17">
+      <c r="A28" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="15">
+        <v>8</v>
+      </c>
+      <c r="H28" s="17">
+        <f>G28</f>
+        <v>8</v>
+      </c>
+      <c r="I28" s="15">
+        <v>26</v>
+      </c>
+      <c r="J28" s="15">
+        <v>61</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="L28" s="20">
+        <f t="shared" si="5"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="M28" s="21" t="str">
+        <f t="shared" si="7"/>
+        <v>160</v>
+      </c>
+      <c r="N28" s="29"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v>"r3.2xlarge" =&gt; 8,</v>
+      </c>
+      <c r="R28" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">r3.2xlarge,8 Cores,$0.7/hour,160 GB, - </v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" s="17" customFormat="1" ht="17">
+      <c r="A29" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="15">
         <v>16</v>
       </c>
-      <c r="I23" s="10">
-        <v>108</v>
-      </c>
-      <c r="J23" s="10">
+      <c r="H29" s="17">
+        <f>G29</f>
+        <v>16</v>
+      </c>
+      <c r="I29" s="15">
+        <v>52</v>
+      </c>
+      <c r="J29" s="15">
+        <v>122</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" s="20">
+        <f t="shared" si="5"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="M29" s="21" t="str">
+        <f t="shared" si="7"/>
+        <v>320</v>
+      </c>
+      <c r="N29" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v>"r3.4xlarge" =&gt; 16,</v>
+      </c>
+      <c r="R29" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">r3.4xlarge,16 Cores,$1.4/hour,320 GB, - </v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="17" customFormat="1" ht="17">
+      <c r="A30" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="B30" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="15">
+        <v>32</v>
+      </c>
+      <c r="H30" s="17">
+        <f>G30</f>
+        <v>32</v>
+      </c>
+      <c r="I30" s="15">
+        <v>104</v>
+      </c>
+      <c r="J30" s="15">
+        <v>244</v>
+      </c>
+      <c r="K30" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="L23" s="13">
+      <c r="L30" s="20">
+        <f t="shared" si="5"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="M30" s="21" t="str">
+        <f t="shared" si="7"/>
+        <v>320</v>
+      </c>
+      <c r="N30" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v>"r3.8xlarge" =&gt; 32,</v>
+      </c>
+      <c r="R30" t="str">
         <f t="shared" si="4"/>
-        <v>0.105</v>
-      </c>
-      <c r="M23" s="25" t="str">
+        <v xml:space="preserve">r3.8xlarge,32 Cores,$2.8/hour,320 GB, - </v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="6" customFormat="1" ht="17">
+      <c r="A31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="10">
+        <v>1</v>
+      </c>
+      <c r="H31" s="6">
+        <v>1</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J31" s="10">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="L31" s="13">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+      <c r="M31" s="23">
+        <v>0</v>
+      </c>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q31" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>320</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="O23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="P23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q23" s="6" t="str">
+        <v>"t1.micro" =&gt; 1,</v>
+      </c>
+      <c r="R31" t="str">
+        <f t="shared" si="4"/>
+        <v>t1.micro,1 Cores,$0.02/hour,0 GB, - Use only for cluster configuration testing</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="17">
+      <c r="A32" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="9">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32" s="7">
+        <v>1</v>
+      </c>
+      <c r="J32" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" s="4">
         <f t="shared" si="5"/>
-        <v>"c3.8xlarge" =&gt; 16,</v>
-      </c>
-      <c r="R23" t="str">
-        <f>E23&amp;","&amp;H23&amp;" Cores,$"&amp;ROUND(B23,2)&amp;"/hour,"&amp;M23&amp;" GB,"&amp;O23&amp;" - "&amp;P23</f>
-        <v>c3.8xlarge,16 Cores,$1.68/hour,320 GB, - Worker Only - Recommended for Worker</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" s="19" customFormat="1" ht="17">
-      <c r="A24" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="18">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="17">
-        <v>2</v>
-      </c>
-      <c r="H24" s="19">
-        <f>G24</f>
-        <v>2</v>
-      </c>
-      <c r="I24" s="17">
-        <v>6.5</v>
-      </c>
-      <c r="J24" s="17">
-        <v>15</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="L24" s="22">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="M32" s="21" t="str">
+        <f t="shared" si="7"/>
+        <v>160</v>
+      </c>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" si="6"/>
+        <v>"m1.small" =&gt; 1,</v>
+      </c>
+      <c r="R32" t="str">
         <f t="shared" si="4"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="M24" s="24" t="str">
-        <f t="shared" si="6"/>
-        <v>32</v>
-      </c>
-      <c r="O24" s="21"/>
-      <c r="Q24" s="19" t="str">
-        <f t="shared" si="5"/>
-        <v>"r3.large" =&gt; 2,</v>
-      </c>
-      <c r="R24" t="str">
-        <f>E24&amp;","&amp;H24&amp;" Cores,$"&amp;ROUND(B24,2)&amp;"/hour,"&amp;M24&amp;" GB,"&amp;O24&amp;" - "&amp;P24</f>
-        <v xml:space="preserve">r3.large,2 Cores,$0.18/hour,32 GB, - </v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" s="19" customFormat="1" ht="17">
-      <c r="A25" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="18">
-        <v>0.35</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="17">
-        <v>4</v>
-      </c>
-      <c r="H25" s="19">
-        <f>G25</f>
-        <v>4</v>
-      </c>
-      <c r="I25" s="17">
-        <v>13</v>
-      </c>
-      <c r="J25" s="17">
-        <v>30.5</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="L25" s="22">
-        <f t="shared" si="4"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="M25" s="24" t="str">
-        <f t="shared" si="6"/>
-        <v>80</v>
-      </c>
-      <c r="O25" s="21"/>
-      <c r="Q25" s="19" t="str">
-        <f t="shared" si="5"/>
-        <v>"r3.xlarge" =&gt; 4,</v>
-      </c>
-      <c r="R25" t="str">
-        <f>E25&amp;","&amp;H25&amp;" Cores,$"&amp;ROUND(B25,2)&amp;"/hour,"&amp;M25&amp;" GB,"&amp;O25&amp;" - "&amp;P25</f>
-        <v xml:space="preserve">r3.xlarge,4 Cores,$0.35/hour,80 GB, - </v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" s="19" customFormat="1" ht="17">
-      <c r="A26" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="17">
-        <v>8</v>
-      </c>
-      <c r="H26" s="19">
-        <f>G26</f>
-        <v>8</v>
-      </c>
-      <c r="I26" s="17">
-        <v>26</v>
-      </c>
-      <c r="J26" s="17">
-        <v>61</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="L26" s="22">
-        <f t="shared" si="4"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="M26" s="24" t="str">
-        <f t="shared" si="6"/>
-        <v>160</v>
-      </c>
-      <c r="O26" s="21"/>
-      <c r="Q26" s="19" t="str">
-        <f t="shared" si="5"/>
-        <v>"r3.2xlarge" =&gt; 8,</v>
-      </c>
-      <c r="R26" t="str">
-        <f>E26&amp;","&amp;H26&amp;" Cores,$"&amp;ROUND(B26,2)&amp;"/hour,"&amp;M26&amp;" GB,"&amp;O26&amp;" - "&amp;P26</f>
-        <v xml:space="preserve">r3.2xlarge,8 Cores,$0.7/hour,160 GB, - </v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" s="19" customFormat="1" ht="17">
-      <c r="A27" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="18">
-        <v>1.4</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="17">
-        <v>16</v>
-      </c>
-      <c r="H27" s="23">
-        <v>16</v>
-      </c>
-      <c r="I27" s="17">
-        <v>52</v>
-      </c>
-      <c r="J27" s="17">
-        <v>122</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L27" s="22">
-        <f t="shared" si="4"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="M27" s="24" t="str">
-        <f t="shared" si="6"/>
-        <v>320</v>
-      </c>
-      <c r="N27" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q27" s="19" t="str">
-        <f t="shared" si="5"/>
-        <v>"r3.4xlarge" =&gt; 16,</v>
-      </c>
-      <c r="R27" t="str">
-        <f>E27&amp;","&amp;H27&amp;" Cores,$"&amp;ROUND(B27,2)&amp;"/hour,"&amp;M27&amp;" GB,"&amp;O27&amp;" - "&amp;P27</f>
-        <v xml:space="preserve">r3.4xlarge,16 Cores,$1.4/hour,320 GB, - </v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" s="19" customFormat="1" ht="17">
-      <c r="A28" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="18">
-        <v>2.8</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="17">
-        <v>32</v>
-      </c>
-      <c r="H28" s="23">
-        <v>32</v>
-      </c>
-      <c r="I28" s="17">
-        <v>104</v>
-      </c>
-      <c r="J28" s="17">
-        <v>244</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="L28" s="22">
-        <f t="shared" si="4"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="M28" s="24" t="str">
-        <f t="shared" si="6"/>
-        <v>320</v>
-      </c>
-      <c r="N28" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q28" s="19" t="str">
-        <f t="shared" si="5"/>
-        <v>"r3.8xlarge" =&gt; 32,</v>
-      </c>
-      <c r="R28" t="str">
-        <f>E28&amp;","&amp;H28&amp;" Cores,$"&amp;ROUND(B28,2)&amp;"/hour,"&amp;M28&amp;" GB,"&amp;O28&amp;" - "&amp;P28</f>
-        <v xml:space="preserve">r3.8xlarge,32 Cores,$2.8/hour,320 GB, - </v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" s="6" customFormat="1" ht="17">
-      <c r="A29" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="11">
-        <v>0.02</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="10">
-        <v>1</v>
-      </c>
-      <c r="H29" s="6">
-        <v>1</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="J29" s="10">
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="K29" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L29" s="13">
-        <f t="shared" si="4"/>
-        <v>0.02</v>
-      </c>
-      <c r="M29" s="25">
-        <v>0</v>
-      </c>
-      <c r="P29" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q29" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>"t1.micro" =&gt; 1,</v>
-      </c>
-      <c r="R29" t="str">
-        <f>E29&amp;","&amp;H29&amp;" Cores,$"&amp;ROUND(B29,2)&amp;"/hour,"&amp;M29&amp;" GB,"&amp;O29&amp;" - "&amp;P29</f>
-        <v>t1.micro,1 Cores,$0.02/hour,0 GB, - Use only for cluster configuration testing</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="17">
-      <c r="A30" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="9">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="7">
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="I30" s="7">
-        <v>1</v>
-      </c>
-      <c r="J30" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L30" s="4">
-        <f t="shared" si="4"/>
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="M30" s="24" t="str">
-        <f t="shared" si="6"/>
-        <v>160</v>
-      </c>
-      <c r="P30" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q30" t="str">
-        <f t="shared" si="5"/>
-        <v>"m1.small" =&gt; 1,</v>
-      </c>
-      <c r="R30" t="str">
-        <f>E30&amp;","&amp;H30&amp;" Cores,$"&amp;ROUND(B30,2)&amp;"/hour,"&amp;M30&amp;" GB,"&amp;O30&amp;" - "&amp;P30</f>
         <v>m1.small,1 Cores,$0.04/hour,160 GB, - Use only for cluster configuration testing</v>
       </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="D1:D14">

</xml_diff>